<commit_message>
added derivation columns (blank) - MB
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_MB.xlsx
+++ b/curation/draft/collection/collection_specialization_MB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884BB64A-A1C0-A147-984A-FBD76B612FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF01BCC1-BB1E-C64C-AD69-CDC35A55B4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="4420" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Collection_MB" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_MB!$A$1:$AH$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_MB!$A$1:$AJ$9</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="109">
   <si>
     <t>package_date</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>categories</t>
+  </si>
+  <si>
+    <t>derived_variable</t>
+  </si>
+  <si>
+    <t>derivation_description</t>
   </si>
 </sst>
 </file>
@@ -770,11 +776,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -786,16 +792,16 @@
     <col min="13" max="13" width="21.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.5" customWidth="1"/>
-    <col min="24" max="24" width="11.83203125" customWidth="1"/>
-    <col min="26" max="26" width="18.5" customWidth="1"/>
-    <col min="27" max="27" width="41.33203125" customWidth="1"/>
-    <col min="28" max="28" width="14.1640625" customWidth="1"/>
-    <col min="29" max="29" width="19" customWidth="1"/>
-    <col min="30" max="30" width="17.83203125" customWidth="1"/>
-    <col min="32" max="32" width="19.6640625" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" customWidth="1"/>
+    <col min="28" max="28" width="18.5" customWidth="1"/>
+    <col min="29" max="29" width="41.33203125" customWidth="1"/>
+    <col min="30" max="30" width="14.1640625" customWidth="1"/>
+    <col min="31" max="31" width="19" customWidth="1"/>
+    <col min="32" max="32" width="17.83203125" customWidth="1"/>
+    <col min="34" max="34" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,40 +872,46 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="32">
+    <row r="2" spans="1:36" ht="32">
       <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
@@ -948,14 +960,14 @@
       <c r="W2" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>53</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="32">
+    <row r="3" spans="1:36" ht="32">
       <c r="B3" s="4" t="s">
         <v>50</v>
       </c>
@@ -1004,14 +1016,14 @@
       <c r="W3" t="s">
         <v>37</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>54</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="32">
+    <row r="4" spans="1:36" ht="32">
       <c r="B4" s="4" t="s">
         <v>50</v>
       </c>
@@ -1060,14 +1072,14 @@
       <c r="W4" t="s">
         <v>35</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>55</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="32">
+    <row r="5" spans="1:36" ht="32">
       <c r="B5" s="4" t="s">
         <v>50</v>
       </c>
@@ -1119,14 +1131,14 @@
       <c r="W5" t="s">
         <v>35</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>56</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AH5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="32">
+    <row r="6" spans="1:36" ht="32">
       <c r="B6" s="4" t="s">
         <v>50</v>
       </c>
@@ -1178,29 +1190,29 @@
       <c r="W6" t="s">
         <v>35</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>44</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>45</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AB6" t="s">
         <v>83</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AC6" t="s">
         <v>84</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AD6" t="s">
         <v>46</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>57</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AH6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="32">
+    <row r="7" spans="1:36" ht="32">
       <c r="B7" s="4" t="s">
         <v>50</v>
       </c>
@@ -1252,26 +1264,26 @@
       <c r="W7" t="s">
         <v>35</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>82</v>
       </c>
-      <c r="Y7" s="3" t="s">
+      <c r="AA7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AE7" t="s">
         <v>77</v>
       </c>
-      <c r="AD7" s="3" t="s">
+      <c r="AF7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>59</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="32">
+    <row r="8" spans="1:36" ht="32">
       <c r="B8" s="4" t="s">
         <v>50</v>
       </c>
@@ -1323,26 +1335,26 @@
       <c r="W8" t="s">
         <v>37</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>80</v>
       </c>
-      <c r="Y8" s="3" t="s">
+      <c r="AA8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AC8" s="3" t="s">
+      <c r="AE8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AD8" s="3" t="s">
+      <c r="AF8" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>60</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="32">
+    <row r="9" spans="1:36" ht="32">
       <c r="B9" s="4" t="s">
         <v>50</v>
       </c>
@@ -1394,14 +1406,14 @@
       <c r="W9" t="s">
         <v>35</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AG9" t="s">
         <v>58</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AH9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="16">
+    <row r="10" spans="1:36" ht="16">
       <c r="B10" s="4" t="s">
         <v>86</v>
       </c>
@@ -1450,14 +1462,14 @@
       <c r="W10" t="s">
         <v>37</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AG10" t="s">
         <v>53</v>
       </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="16">
+    <row r="11" spans="1:36" ht="16">
       <c r="B11" s="4" t="s">
         <v>86</v>
       </c>
@@ -1506,14 +1518,14 @@
       <c r="W11" t="s">
         <v>37</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AG11" t="s">
         <v>54</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AH11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="16">
+    <row r="12" spans="1:36" ht="16">
       <c r="B12" s="4" t="s">
         <v>86</v>
       </c>
@@ -1562,14 +1574,14 @@
       <c r="W12" t="s">
         <v>35</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>55</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AH12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="16">
+    <row r="13" spans="1:36" ht="16">
       <c r="B13" s="4" t="s">
         <v>86</v>
       </c>
@@ -1621,14 +1633,14 @@
       <c r="W13" t="s">
         <v>35</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AG13" t="s">
         <v>56</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AH13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="16">
+    <row r="14" spans="1:36" ht="16">
       <c r="B14" s="4" t="s">
         <v>86</v>
       </c>
@@ -1680,26 +1692,26 @@
       <c r="W14" t="s">
         <v>35</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Z14" t="s">
         <v>44</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
         <v>45</v>
       </c>
-      <c r="AC14" s="3" t="s">
+      <c r="AE14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="AD14" s="3" t="s">
+      <c r="AF14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AG14" t="s">
         <v>57</v>
       </c>
-      <c r="AF14" t="s">
+      <c r="AH14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="16">
+    <row r="15" spans="1:36" ht="16">
       <c r="B15" s="4" t="s">
         <v>86</v>
       </c>
@@ -1751,30 +1763,30 @@
       <c r="W15" t="s">
         <v>35</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Z15" t="s">
         <v>82</v>
       </c>
-      <c r="Y15" s="3" t="s">
+      <c r="AA15" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Z15" s="3" t="s">
+      <c r="AB15" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AC15" t="s">
         <v>97</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AD15" t="s">
         <v>46</v>
       </c>
-      <c r="AD15" s="3"/>
-      <c r="AE15" t="s">
+      <c r="AF15" s="3"/>
+      <c r="AG15" t="s">
         <v>59</v>
       </c>
-      <c r="AF15" t="s">
+      <c r="AH15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="16">
+    <row r="16" spans="1:36" ht="16">
       <c r="B16" s="4" t="s">
         <v>86</v>
       </c>
@@ -1826,26 +1838,26 @@
       <c r="W16" t="s">
         <v>37</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Z16" t="s">
         <v>80</v>
       </c>
-      <c r="Y16" s="3" t="s">
+      <c r="AA16" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="AC16" s="3" t="s">
+      <c r="AE16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AD16" s="3" t="s">
+      <c r="AF16" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AG16" t="s">
         <v>60</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AH16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="2:32" ht="16">
+    <row r="17" spans="2:34" ht="16">
       <c r="B17" s="4" t="s">
         <v>86</v>
       </c>
@@ -1897,22 +1909,22 @@
       <c r="W17" t="s">
         <v>35</v>
       </c>
-      <c r="AE17" t="s">
+      <c r="AG17" t="s">
         <v>58</v>
       </c>
-      <c r="AF17" t="s">
+      <c r="AH17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:32">
-      <c r="Z21" s="3"/>
+    <row r="21" spans="2:34">
+      <c r="AB21" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ9" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="X7" r:id="rId1" xr:uid="{D53504E4-39F9-354E-B337-0329EC62D16D}"/>
-    <hyperlink ref="X15" r:id="rId2" xr:uid="{4332356C-AA9C-3643-8769-D6FAB2A11B44}"/>
+    <hyperlink ref="Z7" r:id="rId1" xr:uid="{D53504E4-39F9-354E-B337-0329EC62D16D}"/>
+    <hyperlink ref="Z15" r:id="rId2" xr:uid="{4332356C-AA9C-3643-8769-D6FAB2A11B44}"/>
     <hyperlink ref="B8" r:id="rId3" xr:uid="{CF162888-5B32-5D46-BC0D-0A5324944807}"/>
     <hyperlink ref="B3:B9" r:id="rId4" display="C198341" xr:uid="{47BB8A3C-CF1C-B040-A8ED-0A35B3A803A5}"/>
     <hyperlink ref="B2" r:id="rId5" xr:uid="{35C55D7B-ADF5-7C42-B36F-C67964CAB269}"/>

</xml_diff>